<commit_message>
Refactor Timer to a single method called by all classifiers
</commit_message>
<xml_diff>
--- a/Wine/Model Comparison.xlsx
+++ b/Wine/Model Comparison.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Myles\PycharmProjects\assignment1test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Myles\Documents\OMSCS\CS7641 ML\Assignment 1\Supervised-Learning\Wine\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>Model</t>
   </si>
@@ -90,14 +90,19 @@
   </si>
   <si>
     <t>alpha: 0.001</t>
+  </si>
+  <si>
+    <t>Runtime in s</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+  <numFmts count="3">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0%"/>
+    <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -132,15 +137,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -454,11 +462,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
+      <selection pane="bottomLeft" activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -470,9 +478,10 @@
     <col min="5" max="5" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -494,8 +503,11 @@
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="H1" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -511,8 +523,11 @@
       <c r="G2" s="1">
         <v>0.51100000000000001</v>
       </c>
+      <c r="H2" s="2">
+        <v>16</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -531,8 +546,11 @@
       <c r="G3" s="1">
         <v>0.53400000000000003</v>
       </c>
+      <c r="H3" s="2">
+        <v>186</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -555,7 +573,7 @@
         <v>0.58199999999999996</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -577,8 +595,11 @@
       <c r="G5" s="1">
         <v>0.63600000000000001</v>
       </c>
+      <c r="H5" s="2">
+        <v>29</v>
+      </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -594,8 +615,11 @@
       <c r="G6" s="1">
         <v>0.63700000000000001</v>
       </c>
+      <c r="H6" s="2">
+        <v>89</v>
+      </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>

</xml_diff>